<commit_message>
changes on test case 105
</commit_message>
<xml_diff>
--- a/testData/BookHotel_TestData/BookHotel1.xlsx
+++ b/testData/BookHotel_TestData/BookHotel1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\webca\eclipse-workspace\seleniumpractice-sept2023\BookHotel_TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k\git\seleniumpractice-sept2023\testData\BookHotel_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7800034E-041F-4A1F-84F0-9233285BF025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FBA7503-097A-4DDE-A41F-2331642E2DBA}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
   </numFmts>
@@ -483,32 +482,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E62B20B-0791-48C0-948A-832357341B87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>